<commit_message>
updated the order of stats in validatefnc in ctdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC04_Canine_StudyOSA01-Breed_Sex_Female.xlsx
+++ b/InputFiles/TC04_Canine_StudyOSA01-Breed_Sex_Female.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Develope_2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4772AFF8-27DB-4389-9D93-E62069705ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11690C2-34CD-4F3A-8C39-F84D5DF8C124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -82,26 +82,6 @@
     count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['OSA01'] and demo.breed in ['Golden Retriever'] and demo.sex in['Female']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE s.clinical_study_designation IN ['OSA01'] and demo.breed in ['Golden Retriever'] and demo.sex in['Female']
  WITH DISTINCT samp AS samp, c, demo, diag
@@ -119,36 +99,86 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['OSA01'] and demo.breed in ['Golden Retriever'] and demo.sex in['Female']
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+ coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
 MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['OSA01'] and demo.breed in ['Golden Retriever'] and demo.sex in['Female']
- WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
+ OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp:sample)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(s:study)
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (f:file)--&gt;(s:study)
 MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['OSA01'] and demo.breed in ['Golden Retriever'] and demo.sex in['Female']
-WITH DISTINCT f, s
-RETURN 
+WITH DISTINCT f,  s, c, demo, diag
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH    
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
   coalesce(f.file_name, '') AS `File Name`,
   coalesce(f.file_type, '') AS `File Type`,
   coalesce("study", '') AS `Association`,
   coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS `File Format`,
-  coalesce(f.file_size, '') AS `Size`,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+</t>
   </si>
 </sst>
 </file>
@@ -529,20 +559,20 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="100" style="1" customWidth="1"/>
-    <col min="3" max="3" width="107.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="63.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="1"/>
+    <col min="3" max="3" width="107.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -559,12 +589,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="376.2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="158.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
@@ -576,12 +606,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="336.6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="255.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -593,7 +623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="336.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="240.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -610,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="297" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -627,7 +657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
     </row>
   </sheetData>

</xml_diff>